<commit_message>
RDM-13079 - categoryid updates for FTAs
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/GenericDefinitionFile.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/GenericDefinitionFile.xlsx
@@ -1,45 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/valid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE3D17-6112-7C4F-B92E-A2DC9BFEC657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF0BD97-B612-A741-A7DD-362FFFD7049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57820" yWindow="800" windowWidth="35840" windowHeight="21940" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
     <sheet name="Banner" sheetId="22" r:id="rId2"/>
     <sheet name="CaseType" sheetId="2" r:id="rId3"/>
-    <sheet name="Category" sheetId="23" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="3" r:id="rId5"/>
-    <sheet name="ComplexTypes" sheetId="4" r:id="rId6"/>
-    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId7"/>
-    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId8"/>
-    <sheet name="FixedLists" sheetId="5" r:id="rId9"/>
-    <sheet name="CaseTypeTab" sheetId="6" r:id="rId10"/>
-    <sheet name="State" sheetId="7" r:id="rId11"/>
-    <sheet name="CaseEvent" sheetId="8" r:id="rId12"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId20"/>
-    <sheet name="CaseRoles" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId23"/>
+    <sheet name="Categories" sheetId="24" r:id="rId4"/>
+    <sheet name="Category" sheetId="23" r:id="rId5"/>
+    <sheet name="CaseField" sheetId="3" r:id="rId6"/>
+    <sheet name="ComplexTypes" sheetId="4" r:id="rId7"/>
+    <sheet name="AuthorisationComplexType" sheetId="21" r:id="rId8"/>
+    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="5" r:id="rId10"/>
+    <sheet name="CaseTypeTab" sheetId="6" r:id="rId11"/>
+    <sheet name="State" sheetId="7" r:id="rId12"/>
+    <sheet name="CaseEvent" sheetId="8" r:id="rId13"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId21"/>
+    <sheet name="CaseRoles" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">CaseEvent!$A$20:$T$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseField!$A$3:$IO$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">CaseEvent!$A$20:$T$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseField!$A$3:$IO$111</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4419" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4459" uniqueCount="819">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2569,6 +2570,31 @@
   </si>
   <si>
     <t>#divorceState</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>From when the configuration is valid</t>
+  </si>
+  <si>
+    <t>Not used - but retained to be consistent with other CCD config</t>
+  </si>
+  <si>
+    <t>CaseTypeId</t>
+  </si>
+  <si>
+    <t>Divorce Sttate</t>
+  </si>
+  <si>
+    <t>translatedDivorceDocs1</t>
+  </si>
+  <si>
+    <t>The Case Type for which the configuration applies
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">te te te te </t>
   </si>
 </sst>
 </file>
@@ -2579,7 +2605,7 @@
     <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;D/&quot;m&quot;/YY&quot;"/>
   </numFmts>
-  <fonts count="59" x14ac:knownFonts="1">
+  <fonts count="60" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2943,9 +2969,16 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333399"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2991,6 +3024,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3159,7 +3198,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="318">
+  <cellXfs count="333">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3960,6 +3999,27 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4003,6 +4063,263 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4070,49 +4387,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4170,6 +4444,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -4177,15 +4460,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -4227,186 +4501,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4418,31 +4512,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="0"/>
+        <color auto="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4477,7 +4551,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color auto="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -4507,7 +4581,160 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0432FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4575,6 +4802,49 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;DD/&quot;mm&quot;/YYYY&quot;"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4687,216 +4957,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0432FF"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -10828,14 +10888,14 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F114" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F114" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10854,40 +10914,40 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="32" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F38" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F38" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F27" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F27" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12190,6 +12250,533 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
+    <col min="3" max="4" width="31.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
+    <col min="8" max="252" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>423</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="70"/>
+    </row>
+    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>250</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>427</v>
+      </c>
+      <c r="F3" s="124" t="s">
+        <v>777</v>
+      </c>
+      <c r="G3" s="73" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>429</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>430</v>
+      </c>
+      <c r="F4" s="129"/>
+      <c r="G4" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>431</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>432</v>
+      </c>
+      <c r="F5" s="129"/>
+      <c r="G5" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>433</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>434</v>
+      </c>
+      <c r="F6" s="129"/>
+      <c r="G6" s="77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="75"/>
+      <c r="C7" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>435</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>436</v>
+      </c>
+      <c r="F7" s="129"/>
+      <c r="G7" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>437</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>438</v>
+      </c>
+      <c r="F8" s="129"/>
+      <c r="G8" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>439</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="129"/>
+      <c r="G9" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>441</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>442</v>
+      </c>
+      <c r="F10" s="129"/>
+      <c r="G10" s="77"/>
+    </row>
+    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="76" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="76" t="s">
+        <v>443</v>
+      </c>
+      <c r="E11" s="76" t="s">
+        <v>444</v>
+      </c>
+      <c r="F11" s="129"/>
+      <c r="G11" s="78"/>
+    </row>
+    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>445</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>446</v>
+      </c>
+      <c r="F12" s="129"/>
+      <c r="G12" s="78"/>
+    </row>
+    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="76" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="76" t="s">
+        <v>447</v>
+      </c>
+      <c r="E13" s="76" t="s">
+        <v>448</v>
+      </c>
+      <c r="F13" s="129"/>
+      <c r="G13" s="77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="79" t="s">
+        <v>449</v>
+      </c>
+      <c r="E14" s="79" t="s">
+        <v>450</v>
+      </c>
+      <c r="F14" s="297"/>
+      <c r="G14" s="78"/>
+    </row>
+    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="79" t="s">
+        <v>451</v>
+      </c>
+      <c r="E15" s="79" t="s">
+        <v>452</v>
+      </c>
+      <c r="F15" s="297"/>
+      <c r="G15" s="78"/>
+    </row>
+    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="82" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" s="82" t="s">
+        <v>453</v>
+      </c>
+      <c r="E16" s="82" t="s">
+        <v>454</v>
+      </c>
+      <c r="F16" s="133"/>
+      <c r="G16" s="77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="81"/>
+      <c r="C17" s="82" t="s">
+        <v>330</v>
+      </c>
+      <c r="D17" s="82" t="s">
+        <v>455</v>
+      </c>
+      <c r="E17" s="82" t="s">
+        <v>456</v>
+      </c>
+      <c r="F17" s="133"/>
+      <c r="G17" s="77"/>
+    </row>
+    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82" t="s">
+        <v>330</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>457</v>
+      </c>
+      <c r="E18" s="82" t="s">
+        <v>458</v>
+      </c>
+      <c r="F18" s="133"/>
+      <c r="G18" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="82" t="s">
+        <v>311</v>
+      </c>
+      <c r="D19" s="82" t="s">
+        <v>459</v>
+      </c>
+      <c r="E19" s="82" t="s">
+        <v>460</v>
+      </c>
+      <c r="F19" s="133"/>
+      <c r="G19" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="82" t="s">
+        <v>311</v>
+      </c>
+      <c r="D20" s="82" t="s">
+        <v>461</v>
+      </c>
+      <c r="E20" s="82" t="s">
+        <v>462</v>
+      </c>
+      <c r="F20" s="133"/>
+      <c r="G20" s="77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="82" t="s">
+        <v>311</v>
+      </c>
+      <c r="D21" s="82" t="s">
+        <v>463</v>
+      </c>
+      <c r="E21" s="82" t="s">
+        <v>464</v>
+      </c>
+      <c r="F21" s="133"/>
+      <c r="G21" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="82" t="s">
+        <v>311</v>
+      </c>
+      <c r="D22" s="82" t="s">
+        <v>465</v>
+      </c>
+      <c r="E22" s="82" t="s">
+        <v>466</v>
+      </c>
+      <c r="F22" s="133"/>
+      <c r="G22" s="77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83" t="s">
+        <v>755</v>
+      </c>
+      <c r="D23" s="79" t="s">
+        <v>756</v>
+      </c>
+      <c r="E23" s="79" t="s">
+        <v>757</v>
+      </c>
+      <c r="F23" s="297"/>
+      <c r="G23" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="85">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86" t="s">
+        <v>755</v>
+      </c>
+      <c r="D24" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E24" s="87" t="s">
+        <v>758</v>
+      </c>
+      <c r="F24" s="298"/>
+      <c r="G24" s="88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B25" s="75"/>
+      <c r="C25" s="79" t="s">
+        <v>803</v>
+      </c>
+      <c r="D25" s="79" t="s">
+        <v>804</v>
+      </c>
+      <c r="E25" s="79" t="s">
+        <v>788</v>
+      </c>
+      <c r="F25" s="297" t="s">
+        <v>787</v>
+      </c>
+      <c r="G25" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="304" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="299">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="300"/>
+      <c r="C26" s="305" t="s">
+        <v>803</v>
+      </c>
+      <c r="D26" s="301" t="s">
+        <v>805</v>
+      </c>
+      <c r="E26" s="301" t="s">
+        <v>806</v>
+      </c>
+      <c r="F26" s="302" t="s">
+        <v>809</v>
+      </c>
+      <c r="G26" s="303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
@@ -13840,7 +14427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
@@ -14364,7 +14951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T34"/>
   <sheetViews>
@@ -15869,7 +16456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q119"/>
   <sheetViews>
@@ -20626,7 +21213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -21385,7 +21972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -21843,7 +22430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -22640,7 +23227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
@@ -23376,7 +23963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -23588,295 +24175,6 @@
   </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId7"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="28" style="13" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="211" t="s">
-        <v>717</v>
-      </c>
-      <c r="B1" s="212" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="213" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="214" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="90"/>
-    </row>
-    <row r="2" spans="1:5" ht="46.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="194" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="194" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="194" t="s">
-        <v>718</v>
-      </c>
-      <c r="D2" s="194" t="s">
-        <v>360</v>
-      </c>
-      <c r="E2" s="194" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>363</v>
-      </c>
-      <c r="E3" s="124" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="76" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E4" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="76" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="95" t="s">
-        <v>720</v>
-      </c>
-      <c r="E5" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E6" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="203" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E7" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="203" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E8" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="203" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E9" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="95"/>
-      <c r="C10" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E10" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="95"/>
-      <c r="C11" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E11" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="95"/>
-      <c r="C12" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E12" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E13" s="129" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="98"/>
-      <c r="C14" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="148" t="s">
-        <v>365</v>
-      </c>
-      <c r="E14" s="133" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="98" t="s">
-        <v>381</v>
-      </c>
-      <c r="E15" s="133" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="98"/>
-      <c r="C16" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="98" t="s">
-        <v>379</v>
-      </c>
-      <c r="E16" s="133" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="85">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="100" t="s">
-        <v>761</v>
-      </c>
-      <c r="D17" s="215" t="s">
-        <v>365</v>
-      </c>
-      <c r="E17" s="139" t="s">
-        <v>364</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -24002,10 +24300,299 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="28" style="13" customWidth="1"/>
+    <col min="6" max="256" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="211" t="s">
+        <v>717</v>
+      </c>
+      <c r="B1" s="212" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="213" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="214" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="90"/>
+    </row>
+    <row r="2" spans="1:5" ht="46.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="194" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="194" t="s">
+        <v>718</v>
+      </c>
+      <c r="D2" s="194" t="s">
+        <v>360</v>
+      </c>
+      <c r="E2" s="194" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" s="124" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="95"/>
+      <c r="C4" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E4" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="95"/>
+      <c r="C5" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="95" t="s">
+        <v>720</v>
+      </c>
+      <c r="E5" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="95"/>
+      <c r="C6" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E6" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="95"/>
+      <c r="C7" s="203" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E7" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="95"/>
+      <c r="C8" s="203" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E8" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="95"/>
+      <c r="C9" s="203" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E9" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="95"/>
+      <c r="C10" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E10" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="95"/>
+      <c r="C11" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E11" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="95"/>
+      <c r="C12" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E12" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B13" s="95"/>
+      <c r="C13" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="129" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B14" s="98"/>
+      <c r="C14" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="148" t="s">
+        <v>365</v>
+      </c>
+      <c r="E14" s="133" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="98"/>
+      <c r="C15" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="98" t="s">
+        <v>381</v>
+      </c>
+      <c r="E15" s="133" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="98"/>
+      <c r="C16" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="98" t="s">
+        <v>379</v>
+      </c>
+      <c r="E16" s="133" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="85">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="104"/>
+      <c r="C17" s="100" t="s">
+        <v>761</v>
+      </c>
+      <c r="D17" s="215" t="s">
+        <v>365</v>
+      </c>
+      <c r="E17" s="139" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -26087,7 +26674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -26206,7 +26793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
@@ -26922,7 +27509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
@@ -27833,11 +28420,258 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A5E75E-0057-1B4D-B48B-CC4925BA5D7C}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="320" t="s">
+        <v>811</v>
+      </c>
+      <c r="B1" s="321"/>
+      <c r="C1" s="322"/>
+      <c r="D1" s="323"/>
+      <c r="E1" s="323"/>
+      <c r="F1" s="323"/>
+      <c r="G1" s="323"/>
+    </row>
+    <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
+      <c r="A2" s="324" t="s">
+        <v>812</v>
+      </c>
+      <c r="B2" s="324" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2" s="324" t="s">
+        <v>817</v>
+      </c>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+    </row>
+    <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="318" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="319" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="318" t="s">
+        <v>814</v>
+      </c>
+      <c r="D3" s="318" t="s">
+        <v>777</v>
+      </c>
+      <c r="E3" s="318" t="s">
+        <v>779</v>
+      </c>
+      <c r="F3" s="318" t="s">
+        <v>428</v>
+      </c>
+      <c r="G3" s="318" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="325">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="325">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="327" t="s">
+        <v>783</v>
+      </c>
+      <c r="E4" s="327" t="s">
+        <v>783</v>
+      </c>
+      <c r="F4" s="326">
+        <v>120</v>
+      </c>
+      <c r="G4" s="326"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="325">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="325">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="327" t="s">
+        <v>793</v>
+      </c>
+      <c r="E5" s="327" t="s">
+        <v>793</v>
+      </c>
+      <c r="F5" s="326">
+        <v>100</v>
+      </c>
+      <c r="G5" s="326"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="325">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="325">
+        <v>42736</v>
+      </c>
+      <c r="C6" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="327" t="s">
+        <v>785</v>
+      </c>
+      <c r="E6" s="327" t="s">
+        <v>786</v>
+      </c>
+      <c r="F6" s="326">
+        <v>110</v>
+      </c>
+      <c r="G6" s="326"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="328">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="328">
+        <v>42736</v>
+      </c>
+      <c r="C7" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="329" t="s">
+        <v>787</v>
+      </c>
+      <c r="E7" s="329" t="s">
+        <v>787</v>
+      </c>
+      <c r="F7" s="323">
+        <v>110</v>
+      </c>
+      <c r="G7" s="329" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="328">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="328">
+        <v>42736</v>
+      </c>
+      <c r="C8" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="329" t="s">
+        <v>789</v>
+      </c>
+      <c r="E8" s="329" t="s">
+        <v>786</v>
+      </c>
+      <c r="F8" s="323">
+        <v>112</v>
+      </c>
+      <c r="G8" s="329" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="328">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="328">
+        <v>42736</v>
+      </c>
+      <c r="C9" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="329" t="s">
+        <v>810</v>
+      </c>
+      <c r="E9" s="329" t="s">
+        <v>815</v>
+      </c>
+      <c r="F9" s="323">
+        <v>113</v>
+      </c>
+      <c r="G9" s="329" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="330">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="330">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="331" t="s">
+        <v>794</v>
+      </c>
+      <c r="E10" s="331" t="s">
+        <v>794</v>
+      </c>
+      <c r="F10" s="332">
+        <v>110</v>
+      </c>
+      <c r="G10" s="331" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="330">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="330">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="326" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="331" t="s">
+        <v>816</v>
+      </c>
+      <c r="E11" s="331" t="s">
+        <v>818</v>
+      </c>
+      <c r="F11" s="332">
+        <v>130</v>
+      </c>
+      <c r="G11" s="331" t="s">
+        <v>787</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="39" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E15BE1-896E-C94F-B2CD-122BE5CAB0E3}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -28082,13 +28916,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IO114"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17:D18"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33388,7 +34222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N65"/>
   <sheetViews>
@@ -35297,7 +36131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A25AD-5D69-564D-9511-0323740C2E1F}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -36073,7 +36907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
@@ -36940,531 +37774,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
-    <col min="3" max="4" width="31.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="4" customWidth="1"/>
-    <col min="8" max="252" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>423</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>424</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>425</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>426</v>
-      </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="70"/>
-    </row>
-    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>250</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>427</v>
-      </c>
-      <c r="F3" s="124" t="s">
-        <v>777</v>
-      </c>
-      <c r="G3" s="73" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="76" t="s">
-        <v>429</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>430</v>
-      </c>
-      <c r="F4" s="129"/>
-      <c r="G4" s="77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>431</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>432</v>
-      </c>
-      <c r="F5" s="129"/>
-      <c r="G5" s="77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>433</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>434</v>
-      </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>435</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>436</v>
-      </c>
-      <c r="F7" s="129"/>
-      <c r="G7" s="77">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="76" t="s">
-        <v>437</v>
-      </c>
-      <c r="E8" s="76" t="s">
-        <v>438</v>
-      </c>
-      <c r="F8" s="129"/>
-      <c r="G8" s="77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="76" t="s">
-        <v>439</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>440</v>
-      </c>
-      <c r="F9" s="129"/>
-      <c r="G9" s="77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="D10" s="76" t="s">
-        <v>441</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>442</v>
-      </c>
-      <c r="F10" s="129"/>
-      <c r="G10" s="77"/>
-    </row>
-    <row r="11" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="76" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="76" t="s">
-        <v>443</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>444</v>
-      </c>
-      <c r="F11" s="129"/>
-      <c r="G11" s="78"/>
-    </row>
-    <row r="12" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="76" t="s">
-        <v>445</v>
-      </c>
-      <c r="E12" s="76" t="s">
-        <v>446</v>
-      </c>
-      <c r="F12" s="129"/>
-      <c r="G12" s="78"/>
-    </row>
-    <row r="13" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="76" t="s">
-        <v>285</v>
-      </c>
-      <c r="D13" s="76" t="s">
-        <v>447</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>448</v>
-      </c>
-      <c r="F13" s="129"/>
-      <c r="G13" s="77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>449</v>
-      </c>
-      <c r="E14" s="79" t="s">
-        <v>450</v>
-      </c>
-      <c r="F14" s="297"/>
-      <c r="G14" s="78"/>
-    </row>
-    <row r="15" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="D15" s="79" t="s">
-        <v>451</v>
-      </c>
-      <c r="E15" s="79" t="s">
-        <v>452</v>
-      </c>
-      <c r="F15" s="297"/>
-      <c r="G15" s="78"/>
-    </row>
-    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="D16" s="82" t="s">
-        <v>453</v>
-      </c>
-      <c r="E16" s="82" t="s">
-        <v>454</v>
-      </c>
-      <c r="F16" s="133"/>
-      <c r="G16" s="77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="D17" s="82" t="s">
-        <v>455</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>456</v>
-      </c>
-      <c r="F17" s="133"/>
-      <c r="G17" s="77"/>
-    </row>
-    <row r="18" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="82" t="s">
-        <v>330</v>
-      </c>
-      <c r="D18" s="82" t="s">
-        <v>457</v>
-      </c>
-      <c r="E18" s="82" t="s">
-        <v>458</v>
-      </c>
-      <c r="F18" s="133"/>
-      <c r="G18" s="77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82" t="s">
-        <v>311</v>
-      </c>
-      <c r="D19" s="82" t="s">
-        <v>459</v>
-      </c>
-      <c r="E19" s="82" t="s">
-        <v>460</v>
-      </c>
-      <c r="F19" s="133"/>
-      <c r="G19" s="77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82" t="s">
-        <v>311</v>
-      </c>
-      <c r="D20" s="82" t="s">
-        <v>461</v>
-      </c>
-      <c r="E20" s="82" t="s">
-        <v>462</v>
-      </c>
-      <c r="F20" s="133"/>
-      <c r="G20" s="77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82" t="s">
-        <v>311</v>
-      </c>
-      <c r="D21" s="82" t="s">
-        <v>463</v>
-      </c>
-      <c r="E21" s="82" t="s">
-        <v>464</v>
-      </c>
-      <c r="F21" s="133"/>
-      <c r="G21" s="77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="82" t="s">
-        <v>311</v>
-      </c>
-      <c r="D22" s="82" t="s">
-        <v>465</v>
-      </c>
-      <c r="E22" s="82" t="s">
-        <v>466</v>
-      </c>
-      <c r="F22" s="133"/>
-      <c r="G22" s="77">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83" t="s">
-        <v>755</v>
-      </c>
-      <c r="D23" s="79" t="s">
-        <v>756</v>
-      </c>
-      <c r="E23" s="79" t="s">
-        <v>757</v>
-      </c>
-      <c r="F23" s="297"/>
-      <c r="G23" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="85">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86" t="s">
-        <v>755</v>
-      </c>
-      <c r="D24" s="87" t="s">
-        <v>759</v>
-      </c>
-      <c r="E24" s="87" t="s">
-        <v>758</v>
-      </c>
-      <c r="F24" s="298"/>
-      <c r="G24" s="88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="79" t="s">
-        <v>803</v>
-      </c>
-      <c r="D25" s="79" t="s">
-        <v>804</v>
-      </c>
-      <c r="E25" s="79" t="s">
-        <v>788</v>
-      </c>
-      <c r="F25" s="297" t="s">
-        <v>787</v>
-      </c>
-      <c r="G25" s="78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="304" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="299">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="300"/>
-      <c r="C26" s="305" t="s">
-        <v>803</v>
-      </c>
-      <c r="D26" s="301" t="s">
-        <v>805</v>
-      </c>
-      <c r="E26" s="301" t="s">
-        <v>806</v>
-      </c>
-      <c r="F26" s="302" t="s">
-        <v>809</v>
-      </c>
-      <c r="G26" s="303">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="G27" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
RDM-13132 - Test data for ComplexTypes FTA tests
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/GenericDefinitionFile.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/GenericDefinitionFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleogeorgiou/Documents/HMCTS-Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF0BD97-B612-A741-A7DD-362FFFD7049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB95B129-434F-B841-8B24-0B7E72AFB0FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="500" windowWidth="35840" windowHeight="20560" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4459" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4458" uniqueCount="818">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2543,9 +2543,6 @@
   </si>
   <si>
     <t>BirthCertificate</t>
-  </si>
-  <si>
-    <t>divorceDocuments</t>
   </si>
   <si>
     <t>divorceState</t>
@@ -12720,10 +12717,10 @@
       </c>
       <c r="B25" s="75"/>
       <c r="C25" s="79" t="s">
+        <v>802</v>
+      </c>
+      <c r="D25" s="79" t="s">
         <v>803</v>
-      </c>
-      <c r="D25" s="79" t="s">
-        <v>804</v>
       </c>
       <c r="E25" s="79" t="s">
         <v>788</v>
@@ -12741,16 +12738,16 @@
       </c>
       <c r="B26" s="300"/>
       <c r="C26" s="305" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D26" s="301" t="s">
+        <v>804</v>
+      </c>
+      <c r="E26" s="301" t="s">
         <v>805</v>
       </c>
-      <c r="E26" s="301" t="s">
-        <v>806</v>
-      </c>
       <c r="F26" s="302" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G26" s="303">
         <v>2</v>
@@ -28423,7 +28420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A5E75E-0057-1B4D-B48B-CC4925BA5D7C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="200" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="200" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -28435,7 +28432,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="320" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B1" s="321"/>
       <c r="C1" s="322"/>
@@ -28446,13 +28443,13 @@
     </row>
     <row r="2" spans="1:7" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="324" t="s">
+        <v>811</v>
+      </c>
+      <c r="B2" s="324" t="s">
         <v>812</v>
       </c>
-      <c r="B2" s="324" t="s">
-        <v>813</v>
-      </c>
       <c r="C2" s="324" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D2" s="324"/>
       <c r="E2" s="324"/>
@@ -28467,7 +28464,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="318" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D3" s="318" t="s">
         <v>777</v>
@@ -28602,10 +28599,10 @@
         <v>28</v>
       </c>
       <c r="D9" s="329" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E9" s="329" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F9" s="323">
         <v>113</v>
@@ -28648,10 +28645,10 @@
         <v>28</v>
       </c>
       <c r="D11" s="331" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E11" s="331" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F11" s="332">
         <v>130</v>
@@ -29926,7 +29923,7 @@
         <v>117</v>
       </c>
       <c r="H18" s="310" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I18" s="309"/>
       <c r="J18" s="309"/>
@@ -34226,8 +34223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35051,12 +35048,10 @@
       <c r="E28" s="314" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="314" t="s">
-        <v>802</v>
-      </c>
+      <c r="F28" s="314"/>
       <c r="G28" s="309"/>
       <c r="H28" s="314" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I28" s="308"/>
       <c r="J28" s="309"/>
@@ -37398,7 +37393,7 @@
         <v>149</v>
       </c>
       <c r="F17" s="316" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G17" s="309"/>
       <c r="H17" s="309"/>

</xml_diff>